<commit_message>
fix: menu contact page & umdate SEO audit
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Lab\OC\p4_hattab_nassim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Lab\OC\p4_hattab_nassim\Starting website\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="945" yWindow="615" windowWidth="27855" windowHeight="17385" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11985" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t>Catégorie</t>
   </si>
@@ -1292,6 +1292,9 @@
     </r>
   </si>
   <si>
+    <t>Performance</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">L'attribut </t>
     </r>
@@ -1331,22 +1334,41 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t>et</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t>utilisation des images de texte.</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Le texte des attributs </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>alt</t>
+      <t xml:space="preserve">Le texte </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>alternatif</t>
     </r>
     <r>
       <rPr>
@@ -1356,6 +1378,200 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> des images ne décrit pas correctement les images et dégrade fortement l'accessibilité aux personnes qui utilisent un lecteur d'écran ou qui ont une connexion lente.</t>
+    </r>
+  </si>
+  <si>
+    <t>Certaines images avec un type de fichier non adapté au Web</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">L'utilisation d'images au format </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>BMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> souvent très volumineuse en taille de fichier impacte les performances et pénalise les utilisateurs avec une connexion lente, le format</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> BMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> n'est pas recommandé, car la prise en charge par les navigateurs est potentiellement limitée, il faut généralement l'éviter pour le contenu web.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/Media/Formats/Image_types</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Les type de fichier recommandé par MDN sont les suivante:
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>APNG:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Pour les animations sans perte de qualité.
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>AVIF:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Un format avec de bonnes performances et sans licence commerciale.
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GIF:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  Pour les images simples et les animations.
+•</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> JPEG: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Un format d'images compressées avec pertes. C'est le format le plus populaire et parmi les mieux pris en charge.
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PNG:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Pourra être préféré à JPEG lorsqu'on a besoin d'une meilleure précision ou de transparence.
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>SVG:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  Un format d'image vectoriel idéal pour les éléments d'interface utilisateur, les icônes ou diagrammes qui nécessitent de s'afficher précisément quelle que soit l'échelle.
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>WebP:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Un excellent choix pour les images statiques ou animées. Les taux de compression de ce format sont meilleurs que pour PNG ou JPEG.</t>
     </r>
   </si>
 </sst>
@@ -1477,7 +1693,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1524,6 +1740,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2002,10 +2221,10 @@
         <v>39</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>54</v>
@@ -2017,13 +2236,25 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="2"/>
+    <row r="13" spans="1:26" ht="207" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
@@ -3150,8 +3381,9 @@
     <hyperlink ref="F7" r:id="rId9"/>
     <hyperlink ref="F6" r:id="rId10"/>
     <hyperlink ref="F11" r:id="rId11" location="fallbacks"/>
+    <hyperlink ref="F13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId12"/>
+  <pageSetup orientation="landscape" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update SEO audit
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
   <si>
     <t>Catégorie</t>
   </si>
@@ -355,41 +355,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> est complètement vide, et ne fournit aucune description aux moteurs de recherche et aux utilisateurs lors des résultats au sein des SERP.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Utilisez toujours un attribut</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>lang</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> sur l’élément html. Il sera hérité par tous les autres éléments, et ainsi il fixera la langue par défaut de tout le texte.</t>
     </r>
   </si>
   <si>
@@ -1177,8 +1142,378 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Il est très important que le texte du lien ait un sens.Le texte du lien doit à lui seul transmettre la fonction et le but du lien. Il doit également être unique et facile à exprimer à haute voix. Il faut tenir compte des ces directives lors de la rédaction du texte du lens:                                                                                           </t>
+    <t xml:space="preserve"> Accessibilité</t>
+  </si>
+  <si>
+    <t>Le texte du lien vers la page contact n'explique pas clairement la fonction et le but du lien. Cela conduit à une dégradation de l'expérience utilisateur et nuit de manière significative  l'accessibilité pour les utilisateurs des lecteurs d'écran.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">L'attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">alt </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">doit être présent sur toutes les images, il est </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>incroyablement utile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> pour l'accessibilité, les lecteurs d'écran lisent cette description à leurs utilisateurs pour qu'ils sachent ce que signifie l'image. Le texte </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>alt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> est également affiché sur la page si l'image ne peut pas être chargée pour une raison quelconque : par exemple, erreurs de réseau, blocage du contenu ou linkrot. Également, selon WCAG, si l'utilisation du texte permet d'obtenir le même effet visuel ex (texte sur une image) alors on doit présenter les informations sous forme de texte plutôt que d'utiliser une image.</t>
+    </r>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">L'utilisation d'images au format </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>BMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> souvent très volumineuse en taille de fichier impacte les performances et pénalise les utilisateurs avec une connexion lente, le format</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> BMP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> n'est pas recommandé, car la prise en charge par les navigateurs est potentiellement limitée, il faut généralement l'éviter pour le contenu web.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/Media/Formats/Image_types</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Les type de fichier recommandé par MDN sont les suivante:
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>APNG:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Pour les animations sans perte de qualité.
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>AVIF:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Un format avec de bonnes performances et sans licence commerciale.
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GIF:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  Pour les images simples et les animations.
+•</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> JPEG: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Un format d'images compressées avec pertes. C'est le format le plus populaire et parmi les mieux pris en charge.
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PNG:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Pourra être préféré à JPEG lorsqu'on a besoin d'une meilleure précision ou de transparence.
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>SVG:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  Un format d'image vectoriel idéal pour les éléments d'interface utilisateur, les icônes ou diagrammes qui nécessitent de s'afficher précisément quelle que soit l'échelle.
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>WebP:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Un excellent choix pour les images statiques ou animées. Les taux de compression de ce format sont meilleurs que pour PNG ou JPEG.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Utilisez toujours un attribut</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>lang</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> sur l’élément html pour déclarer la langue du texte par défaut dans la page. Il sera hérité par tous les autres éléments, et ainsi il fixera la langue par défaut de tout le texte. Quand la page contient du contenu dans une autre langue, ajoutez un attribut de langue à un élément qui encadre ce contenu. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">L'attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">atl </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">sur les balises </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">img, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>et</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>utilisation des</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> images de texte.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Il est très important que le texte du lien ait un sens.Le texte du lien doit à lui seul transmettre la fonction et le but du lien. Il doit également être unique et facile à exprimer à haute voix. Il faut tenir compte des ces directives lors de la rédaction du texte du lens:                                                                                           
+</t>
     </r>
     <r>
       <rPr>
@@ -1224,139 +1559,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> Accessibilité</t>
-  </si>
-  <si>
-    <t>Le texte du lien vers la page contact n'explique pas clairement la fonction et le but du lien. Cela conduit à une dégradation de l'expérience utilisateur et nuit de manière significative  l'accessibilité pour les utilisateurs des lecteurs d'écran.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">L'attribut </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">alt </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">doit être présent sur toutes les images, il est </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>incroyablement utile</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> pour l'accessibilité, les lecteurs d'écran lisent cette description à leurs utilisateurs pour qu'ils sachent ce que signifie l'image. Le texte </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>alt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> est également affiché sur la page si l'image ne peut pas être chargée pour une raison quelconque : par exemple, erreurs de réseau, blocage du contenu ou linkrot. Également, selon WCAG, si l'utilisation du texte permet d'obtenir le même effet visuel ex (texte sur une image) alors on doit présenter les informations sous forme de texte plutôt que d'utiliser une image.</t>
-    </r>
-  </si>
-  <si>
-    <t>Performance</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">L'attribut </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">atl </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">sur les balises </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">img, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>et</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>utilisation des images de texte.</t>
-    </r>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Le texte </t>
     </r>
@@ -1377,201 +1579,200 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> des images ne décrit pas correctement les images et dégrade fortement l'accessibilité aux personnes qui utilisent un lecteur d'écran ou qui ont une connexion lente.</t>
-    </r>
-  </si>
-  <si>
-    <t>Certaines images avec un type de fichier non adapté au Web</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">L'utilisation d'images au format </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>BMP</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> souvent très volumineuse en taille de fichier impacte les performances et pénalise les utilisateurs avec une connexion lente, le format</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> BMP</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> n'est pas recommandé, car la prise en charge par les navigateurs est potentiellement limitée, il faut généralement l'éviter pour le contenu web.</t>
-    </r>
-  </si>
-  <si>
-    <t>https://developer.mozilla.org/fr/docs/Web/Media/Formats/Image_types</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Les type de fichier recommandé par MDN sont les suivante:
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>APNG:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Pour les animations sans perte de qualité.
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>AVIF:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Un format avec de bonnes performances et sans licence commerciale.
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>GIF:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  Pour les images simples et les animations.
-•</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> JPEG: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Un format d'images compressées avec pertes. C'est le format le plus populaire et parmi les mieux pris en charge.
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>PNG:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Pourra être préféré à JPEG lorsqu'on a besoin d'une meilleure précision ou de transparence.
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>SVG:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  Un format d'image vectoriel idéal pour les éléments d'interface utilisateur, les icônes ou diagrammes qui nécessitent de s'afficher précisément quelle que soit l'échelle.
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>WebP:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Un excellent choix pour les images statiques ou animées. Les taux de compression de ce format sont meilleurs que pour PNG ou JPEG.</t>
+      <t xml:space="preserve"> des images ne décrit pas correctement les images et dégrade fortement l'accessibilité aux personnes qui utilisent un lecteur d'écran ou qui ont une connexion lente. Également, les images de texte sortent de l'écran sur les resolutions mobile. Une fois redimensionnée pour les adapter aux petites résolutions, le texte devient illisible.</t>
+    </r>
+  </si>
+  <si>
+    <t>La présentation visuelle de certains elements texte ne fousrnissent pas suffisament de contraste entre le texte et son arrière-plan pour qu'il puisse être lu par des personnes ayant une vision modérément basse.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">La présentation visuelle du texte et des images de texte a un rapport de contraste d'au moins 4,5:1, à l'exception des éléments suivants :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Texte de grande taille</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Le texte à grande échelle et les images de texte à grande échelle ont un rapport de contraste d'au moins 3:1 ;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Accessoire</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Le texte ou les images de texte qui font partie d'un composant d'interface utilisateur inactif , qui sont purement décoratifs , qui ne sont visibles par personne, ou qui font partie d'une image qui contient un autre contenu visuel significatif, n'ont aucune exigence de contraste.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Logotypes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Le texte qui fait partie d'un logo ou d'un nom de marque n'a aucune exigence de contraste.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Le </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ratio de contraste </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sur certains elements texte</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Certaines </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>images avec un type de fichier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> non adapté au Web</t>
+    </r>
+  </si>
+  <si>
+    <t>https://web.dev/labels-and-text-alternatives/#label-buttons-and-links</t>
+  </si>
+  <si>
+    <r>
+      <t>Les</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> liens des réseaux sociaux </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">dans le </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>footer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> ne contient aucun nom ou description accessible</t>
+    </r>
+  </si>
+  <si>
+    <t>les utilisateurs de lecteur d'écran n'ont aucune description des liens symbolisés par une icône qui ne contient aucun nom ou description.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dans le cadre d'utilisation des liens ou des buttons présenté visuellement par des icônes ou des images, il est recommandé d'ajouter un attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>aria-label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> pour donner une description de la fonction du lien.</t>
     </r>
   </si>
 </sst>
@@ -1962,13 +2163,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
     <col min="2" max="2" width="27.88671875" customWidth="1"/>
     <col min="3" max="3" width="62.109375" customWidth="1"/>
     <col min="4" max="4" width="91.88671875" customWidth="1"/>
@@ -2025,10 +2226,10 @@
         <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>10</v>
@@ -2045,10 +2246,10 @@
         <v>17</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="4" t="s">
@@ -2066,7 +2267,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>10</v>
@@ -2083,10 +2284,10 @@
         <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>10</v>
@@ -2098,36 +2299,36 @@
     </row>
     <row r="6" spans="1:26" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>10</v>
@@ -2187,7 +2388,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>10</v>
@@ -2198,36 +2399,36 @@
     </row>
     <row r="11" spans="1:26" ht="166.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>10</v>
@@ -2238,39 +2439,63 @@
     </row>
     <row r="13" spans="1:26" ht="207" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="2"/>
+    <row r="14" spans="1:26" ht="184.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+    <row r="15" spans="1:26" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
@@ -3382,8 +3607,10 @@
     <hyperlink ref="F6" r:id="rId10"/>
     <hyperlink ref="F11" r:id="rId11" location="fallbacks"/>
     <hyperlink ref="F13" r:id="rId12"/>
+    <hyperlink ref="F14" r:id="rId13"/>
+    <hyperlink ref="F15" r:id="rId14" location="label-buttons-and-links"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId13"/>
+  <pageSetup orientation="landscape" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: SEO audit sorted by importance
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -74,12 +74,6 @@
     <t>https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links</t>
   </si>
   <si>
-    <t>Utilisation de texte ou de lien cachés en vue de manipuler le classement dans les résultats de recherche est considérée comme une technique trompeuse par Google, et les pages peuvent être supprimé des résultats de recherche.</t>
-  </si>
-  <si>
-    <t>Utilisation des mots-clés cachés, text blanc sur un fond blanc avec la taille de police sur 1px.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">La balise </t>
     </r>
@@ -1991,6 +1985,33 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> est aussi un facteur à ne pas négliger, celle-ci ne doit pas être sur-optimisée. Celui-ci doit être cohérent avec la page vers laquelle il pointe, cependant attention à ne pas utiliser toujours la même ancre par exemple.</t>
+    </r>
+  </si>
+  <si>
+    <t>Utilisation de texte et des liens en tentant de les dissimuler en vue de manipuler le classement dans les résultats de recherche est considérée comme une technique trompeuse par Google, et les pages peuvent être supprimé des résultats de recherche.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Utilisation des </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mots-clés cachés</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, text gris clair sur un fond blanc avec la taille de police sur 1px.</t>
     </r>
   </si>
 </sst>
@@ -2112,13 +2133,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -2144,9 +2162,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2379,10 +2394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2397,22 +2412,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1"/>
@@ -2437,298 +2452,298 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="152.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="4" t="s">
-        <v>7</v>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+    <row r="5" spans="1:26" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="152.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="B5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="16"/>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="A6" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="207" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="5" t="s">
+    </row>
+    <row r="9" spans="1:26" ht="153" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="166.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="B10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="184.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="3" t="s">
+    </row>
+    <row r="13" spans="1:26" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="160.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="D14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+    <row r="15" spans="1:26" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:26" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="160.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="C16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="166.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="207" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="184.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>72</v>
+      <c r="E16" s="6"/>
+      <c r="F16" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -2736,7 +2751,7 @@
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -2744,7 +2759,7 @@
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -2752,7 +2767,7 @@
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -2760,7 +2775,7 @@
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
+      <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -2768,7 +2783,7 @@
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
+      <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2776,7 +2791,7 @@
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
+      <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -2784,7 +2799,7 @@
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
+      <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -2792,7 +2807,7 @@
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
+      <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -2807,46 +2822,11 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3810,30 +3790,23 @@
     <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="F3" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F8" r:id="rId5"/>
-    <hyperlink ref="F10" r:id="rId6"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F15" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId4"/>
+    <hyperlink ref="F5" r:id="rId5"/>
+    <hyperlink ref="F14" r:id="rId6"/>
     <hyperlink ref="F9" r:id="rId7"/>
-    <hyperlink ref="F12" r:id="rId8"/>
-    <hyperlink ref="F7" r:id="rId9"/>
-    <hyperlink ref="F6" r:id="rId10"/>
-    <hyperlink ref="F11" r:id="rId11" location="fallbacks"/>
-    <hyperlink ref="F13" r:id="rId12"/>
-    <hyperlink ref="F14" r:id="rId13"/>
-    <hyperlink ref="F15" r:id="rId14" location="label-buttons-and-links"/>
-    <hyperlink ref="F16" r:id="rId15"/>
+    <hyperlink ref="F7" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9" location="fallbacks"/>
+    <hyperlink ref="F8" r:id="rId10"/>
+    <hyperlink ref="F11" r:id="rId11"/>
+    <hyperlink ref="F13" r:id="rId12" location="label-buttons-and-links"/>
+    <hyperlink ref="F12" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId16"/>
+  <pageSetup orientation="landscape" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>